<commit_message>
[2.2.2.1] Add ГОСТ Р 51613-2000
</commit_message>
<xml_diff>
--- a/AddingToDb.xlsx
+++ b/AddingToDb.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E68761-A33C-4A21-BCDF-3B006BC86C12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD17C64-F34A-4364-B49E-63374A5AEADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Id</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Версия БД 2.2.1.0</t>
+  </si>
+  <si>
+    <t>ГОСТ Р 51613-2000</t>
+  </si>
+  <si>
+    <t>Трубы напорные из непластифицированного поливинилхлорида. Технические условия</t>
+  </si>
+  <si>
+    <t>Версия БД 2.2.2.1</t>
   </si>
 </sst>
 </file>
@@ -205,10 +214,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -551,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,11 +581,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -587,11 +599,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -716,11 +728,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -807,11 +819,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -838,6 +850,22 @@
       </c>
       <c r="C25" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement IDbSection. Add tests
</commit_message>
<xml_diff>
--- a/AddingToDb.xlsx
+++ b/AddingToDb.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD17C64-F34A-4364-B49E-63374A5AEADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1322B08E-309F-4932-91BC-913F83966AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,7 +566,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>